<commit_message>
update goods price in seed;
</commit_message>
<xml_diff>
--- a/database/goods.xlsx
+++ b/database/goods.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxiaopei/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxiaopei/work/huayan2/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11C46F7B-1C47-7B49-9B3D-F4DFAC917BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F7D63E-9C31-674B-8DC5-9582791306EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1420" windowWidth="27240" windowHeight="14940" xr2:uid="{318EE4C6-ECB0-EE48-905F-0535CD2B463E}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,7 +571,7 @@
         <v>21</v>
       </c>
       <c r="E4">
-        <v>188</v>
+        <v>0.02</v>
       </c>
       <c r="F4">
         <v>338</v>
@@ -597,7 +597,7 @@
         <v>15</v>
       </c>
       <c r="E5">
-        <v>29</v>
+        <v>0.01</v>
       </c>
       <c r="F5">
         <v>59</v>

</xml_diff>

<commit_message>
add stock/item; add status to user, and check it in api;
</commit_message>
<xml_diff>
--- a/database/goods.xlsx
+++ b/database/goods.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxiaopei/work/huayan2/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangxiaopei/work/huayan2/public/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F7D63E-9C31-674B-8DC5-9582791306EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821D55FE-B013-384F-A658-35D47468A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1420" windowWidth="27240" windowHeight="14940" xr2:uid="{318EE4C6-ECB0-EE48-905F-0535CD2B463E}"/>
+    <workbookView xWindow="1560" yWindow="1380" windowWidth="27240" windowHeight="14940" xr2:uid="{318EE4C6-ECB0-EE48-905F-0535CD2B463E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>上架</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>本博</t>
+  </si>
+  <si>
+    <t>采购价</t>
   </si>
 </sst>
 </file>
@@ -462,19 +465,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69A92CF-7943-7648-A708-EF841FF2EC6F}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -494,16 +497,19 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -523,14 +529,17 @@
         <v>239</v>
       </c>
       <c r="G2">
+        <v>88</v>
+      </c>
+      <c r="H2">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -550,14 +559,17 @@
         <v>32.799999999999997</v>
       </c>
       <c r="G3">
+        <v>6.8</v>
+      </c>
+      <c r="H3">
         <v>20</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -577,13 +589,16 @@
         <v>338</v>
       </c>
       <c r="G4">
+        <v>0.01</v>
+      </c>
+      <c r="H4">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -603,12 +618,15 @@
         <v>59</v>
       </c>
       <c r="G5">
+        <v>0.01</v>
+      </c>
+      <c r="H5">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>